<commit_message>
Added basic README, added user input to close in prep for .exe release. Forgot to remove quotes.txt.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,10 +14,10 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1641523961" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1641523961" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1641523961" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1641523961"/>
+      <pm:revision xmlns:pm="smNativeData" day="1641524306" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1641524306" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1641524306" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1641524306"/>
     </ext>
   </extLst>
 </workbook>
@@ -69,7 +69,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641523961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641524306" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -102,7 +102,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641523961"/>
+          <pm:border xmlns:pm="smNativeData" id="1641524306"/>
         </ext>
       </extLst>
     </border>
@@ -119,7 +119,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1641523961" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1641524306" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -430,7 +430,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1641523961" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641524306" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -439,16 +439,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1641523961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1641523961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1641523961" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1641523961" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1641524306" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641524306" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641524306" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641524306" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641523961" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641524306" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -470,14 +470,11 @@
     <row r="1" spans="1:1">
       <c r="A1"/>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2"/>
-    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1641523961" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641524306" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -486,16 +483,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1641523961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1641523961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1641523961" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1641523961" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1641524306" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641524306" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641524306" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641524306" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641523961" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641524306" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>